<commit_message>
uppdaterat Elsevier, Sage, IOS
</commit_message>
<xml_diff>
--- a/Bibsam_tidskriftslistor/scifree_data_ios_discount.xlsx
+++ b/Bibsam_tidskriftslistor/scifree_data_ios_discount.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1862,18 +1862,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1919,7 +1921,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1942,7 +1944,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +2013,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2036,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2059,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2103,7 +2105,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2172,7 +2174,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2195,7 +2197,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2218,7 +2220,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2310,7 +2312,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2379,7 +2381,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +2404,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2425,7 +2427,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2448,7 +2450,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2514,7 +2516,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2537,7 +2539,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2560,7 +2562,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2583,7 +2585,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2606,7 +2608,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2629,7 +2631,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2744,7 +2746,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2767,7 +2769,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2787,7 +2789,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2812,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2827,13 +2829,13 @@
         <v>418</v>
       </c>
       <c r="F42" t="s">
-        <v>0</v>
+        <v>502</v>
       </c>
       <c r="G42" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2879,7 +2881,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2902,7 +2904,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2925,7 +2927,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2948,7 +2950,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2994,7 +2996,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -3017,7 +3019,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -3040,7 +3042,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3063,7 +3065,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -3086,7 +3088,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -3155,7 +3157,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -3178,7 +3180,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -3201,7 +3203,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3247,7 +3249,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3293,7 +3295,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -3316,7 +3318,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3362,7 +3364,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3385,7 +3387,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3410,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3431,7 +3433,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -3500,7 +3502,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -3523,7 +3525,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -3546,7 +3548,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -3569,7 +3571,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -3592,7 +3594,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -3615,7 +3617,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -3684,7 +3686,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3707,7 +3709,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -3730,7 +3732,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -3753,7 +3755,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -3776,7 +3778,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3799,7 +3801,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -3868,7 +3870,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -3914,7 +3916,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -3937,7 +3939,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -3960,7 +3962,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -3983,7 +3985,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -4006,7 +4008,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -4029,7 +4031,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -4098,7 +4100,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -4144,7 +4146,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -4167,7 +4169,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -4190,7 +4192,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -4236,7 +4238,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -4259,7 +4261,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -4328,7 +4330,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4353,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -4374,7 +4376,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -4420,7 +4422,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -4443,7 +4445,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -4466,7 +4468,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -4489,7 +4491,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -4512,7 +4514,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -4535,7 +4537,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -4558,7 +4560,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -4581,7 +4583,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -4604,7 +4606,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -4650,7 +4652,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -4673,7 +4675,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -4696,7 +4698,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -4719,7 +4721,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>8</v>
       </c>

</xml_diff>